<commit_message>
Atualização automática de NONOAI.xlsx
</commit_message>
<xml_diff>
--- a/NONOAI.xlsx
+++ b/NONOAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{105C4D7C-B350-49D4-847B-EFFE940057A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B34B91-6548-453F-A8BB-9DF5A9E2210E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1218,7 +1205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1279,30 +1266,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1320,7 +1283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1359,17 +1322,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1416,7 +1374,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{FF117790-4948-404E-8C41-378C3A7BC53F}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4ACF804E-8CE3-4EB2-A61F-F81EC66092E9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1446,10 +1404,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135AF619-B974-4DB7-BF45-3E78B318BD99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DAB5298-1EA2-47C3-8782-2AA5A33C5950}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1487,7 +1445,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0A6A491-CFD3-48B9-89DF-C8EB0A0D9E17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3333047-D37F-47AF-B682-C0FBEC946794}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1550,7 +1508,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{351775A2-DB4C-4C8F-868F-FE89A62EDF54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95374C21-092A-4C35-A522-CAC36F878372}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1569,7 +1527,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF03F3E8-C16C-F255-9213-7AF8A4A25B29}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA18CB3-8A67-8750-0EB3-B6765367AA2D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1618,7 +1576,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12DE7C25-20BB-7225-E771-5400FE63DA3B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02E698E-C3B8-EB83-93B3-36BE84EC9C85}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1637,7 +1595,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51BE3478-0F8C-EBA0-8435-E84A15AFC0D4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CE49FA1-85FA-5CAF-8FE8-705B042937C0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1668,7 +1626,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F369F0DF-4DF4-754B-CE75-0E6A71AD0F9A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{732B35BF-0468-54F2-D61F-B972491FD174}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1699,7 +1657,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A214E067-8825-45EA-8A49-6B7C51EA4134}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CDEF7A-CB47-56AE-3119-0F827994224C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1742,7 +1700,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44454BD4-77E1-4C89-B9F5-80858C9897E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35D0B555-7E4D-4C8A-B17F-D6719CF9D9C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1780,7 +1738,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D97FDF7-4586-4D98-A126-9C0463B7B1E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B447E196-087D-40B1-A709-7126C7B3670B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1823,7 +1781,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BC6977-059F-4694-87AA-229F8075DB4A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD1EB63-D3F3-443F-8A17-4E5515E9B224}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2136,7 +2094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BA5088-4BC7-4959-8E5A-46360975C8E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89CEBE2-F646-451B-A021-99F72FB611EB}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2148,98 +2106,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5503,19 +5461,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5549,46 +5507,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5596,7 +5554,7 @@
       <c r="A2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>398713</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5608,10 +5566,10 @@
       <c r="E2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>33.11</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>331.08</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5640,7 +5598,7 @@
       <c r="A3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>453129</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5652,10 +5610,10 @@
       <c r="E3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>498.71</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>690</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5684,7 +5642,7 @@
       <c r="A4" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>453130</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5696,10 +5654,10 @@
       <c r="E4" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>1365.71</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>1890</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5728,7 +5686,7 @@
       <c r="A5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>453131</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5740,10 +5698,10 @@
       <c r="E5" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>3822.21</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>5290</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5772,7 +5730,7 @@
       <c r="A6" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>453132</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5784,10 +5742,10 @@
       <c r="E6" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>1749.5</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>3599</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5816,7 +5774,7 @@
       <c r="A7" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>461499</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5828,10 +5786,10 @@
       <c r="E7" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>1065.18</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>1299</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5860,7 +5818,7 @@
       <c r="A8" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>463097</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5872,10 +5830,10 @@
       <c r="E8" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>266.64999999999998</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>416.41</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5904,7 +5862,7 @@
       <c r="A9" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>463098</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5916,10 +5874,10 @@
       <c r="E9" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>376.26</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>458.82</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -5948,7 +5906,7 @@
       <c r="A10" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>455393</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -5960,10 +5918,10 @@
       <c r="E10" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>386.4</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>466.9</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -5992,7 +5950,7 @@
       <c r="A11" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>455205</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6004,10 +5962,10 @@
       <c r="E11" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>280.83999999999997</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>419</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6036,7 +5994,7 @@
       <c r="A12" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>455245</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6048,10 +6006,10 @@
       <c r="E12" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>876.22</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>1279</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6080,7 +6038,7 @@
       <c r="A13" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>581327</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6092,10 +6050,10 @@
       <c r="E13" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>590.54</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>595</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6124,7 +6082,7 @@
       <c r="A14" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>581688</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6136,10 +6094,10 @@
       <c r="E14" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>416.41</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>416.41</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6178,14 +6136,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>323</v>
       </c>
     </row>
@@ -6216,46 +6174,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>329</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>327</v>
       </c>
     </row>
@@ -6280,54 +6238,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>340</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>343</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>344</v>
       </c>
     </row>
@@ -6338,43 +6297,43 @@
       <c r="B2" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45352</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>1747</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>6337</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>825</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>348</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>349</v>
       </c>
     </row>
@@ -6405,25 +6364,24 @@
       <c r="B1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="36">
         <v>31</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" s="39">
-        <v>31</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>2.0499933871181062E-3</v>
       </c>
     </row>

</xml_diff>